<commit_message>
Final commit Irene 05/05/2015
</commit_message>
<xml_diff>
--- a/Docs/5_Data Base Tables And Inserts/Tables_and_Inserts.xlsx
+++ b/Docs/5_Data Base Tables And Inserts/Tables_and_Inserts.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="226">
   <si>
     <t>USERS</t>
   </si>
@@ -700,6 +700,15 @@
   <si>
     <t>Singer-songwriter</t>
   </si>
+  <si>
+    <t>Vinyl</t>
+  </si>
+  <si>
+    <t>Cassette</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
 </sst>
 </file>
 
@@ -887,6 +896,8 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -899,8 +910,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1222,16 +1231,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
@@ -1660,12 +1669,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:6">
@@ -1715,11 +1724,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:5">
@@ -1760,12 +1769,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:6">
@@ -1814,10 +1823,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -1862,11 +1871,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:5">
@@ -1911,10 +1920,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -1958,10 +1967,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
@@ -2025,11 +2034,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:5">
@@ -2075,11 +2084,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">
@@ -27103,10 +27112,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
@@ -27442,13 +27451,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="12" t="s">
@@ -27504,8 +27513,8 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -27517,18 +27526,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="11" t="s">
@@ -27572,8 +27581,8 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>224</v>
       </c>
       <c r="D3" t="s">
         <v>125</v>
@@ -27597,8 +27606,8 @@
         <v>1</v>
       </c>
       <c r="L3" t="str">
-        <f>CONCATENATE("INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(",B3,",",C3,",'",D3,"','",E3,"',",F3,",'",G3,"','",H3,"','",I3,"',",J3,")")</f>
-        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(1,0,'Veneno en la piel','Radio Futura',1990,'1','2','img/items/item0.jpg',1)</v>
+        <f>CONCATENATE("INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(",B3,",'",C3,"','",D3,"','",E3,"',",F3,",'",G3,"','",H3,"','",I3,"',",J3,")")</f>
+        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(1,'Cassette','Veneno en la piel','Radio Futura',1990,'1','2','img/items/item0.jpg',1)</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -27608,8 +27617,8 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>224</v>
       </c>
       <c r="D4" t="s">
         <v>137</v>
@@ -27633,8 +27642,8 @@
         <v>1</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L11" si="0">CONCATENATE("INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(",B4,",",C4,",'",D4,"','",E4,"',",F4,",'",G4,"','",H4,"','",I4,"',",J4,")")</f>
-        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(2,0,'No es pecado','Alaska y Dinarama',1986,'0','1','img/items/item1.jpg',1)</v>
+        <f t="shared" ref="L4:L11" si="0">CONCATENATE("INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(",B4,",'",C4,"','",D4,"','",E4,"',",F4,",'",G4,"','",H4,"','",I4,"',",J4,")")</f>
+        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(2,'Cassette','No es pecado','Alaska y Dinarama',1986,'0','1','img/items/item1.jpg',1)</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -27644,8 +27653,8 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>224</v>
       </c>
       <c r="D5" t="s">
         <v>138</v>
@@ -27670,7 +27679,7 @@
       </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(3,0,'Lo mejor de…','Leño',1990,'1','2','img/items/item2.jpg',1)</v>
+        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(3,'Cassette','Lo mejor de…','Leño',1990,'1','2','img/items/item2.jpg',1)</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -27680,8 +27689,8 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>1</v>
+      <c r="C6" t="s">
+        <v>223</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>140</v>
@@ -27706,7 +27715,7 @@
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(1,1,'The very best of','Enya',2009,'9','0','img/items/item3.jpg',1)</v>
+        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(1,'Vinyl','The very best of','Enya',2009,'9','0','img/items/item3.jpg',1)</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -27716,8 +27725,8 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7">
-        <v>1</v>
+      <c r="C7" t="s">
+        <v>223</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>142</v>
@@ -27742,7 +27751,7 @@
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(2,1,'Rumours','Fleetwood Mac',1977,'1','1','img/items/item4.jpg',1)</v>
+        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(2,'Vinyl','Rumours','Fleetwood Mac',1977,'1','1','img/items/item4.jpg',1)</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -27752,8 +27761,8 @@
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="C8" t="s">
+        <v>223</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>145</v>
@@ -27778,7 +27787,7 @@
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(4,1,'Chariots of fire','Vangelis',1981,'11','1','img/items/item5.jpg',1)</v>
+        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(4,'Vinyl','Chariots of fire','Vangelis',1981,'11','1','img/items/item5.jpg',1)</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -27788,8 +27797,8 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9">
-        <v>2</v>
+      <c r="C9" t="s">
+        <v>225</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>146</v>
@@ -27814,7 +27823,7 @@
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(1,2,'Kvelertak','Kvelertak',2010,'7','0','img/items/item6.jpg',1)</v>
+        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(1,'CD','Kvelertak','Kvelertak',2010,'7','0','img/items/item6.jpg',1)</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -27824,8 +27833,8 @@
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>2</v>
+      <c r="C10" t="s">
+        <v>225</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>148</v>
@@ -27850,7 +27859,7 @@
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(9,2,'19 días y 500 noches','Joaquín Sabina',1990,'10','2','img/items/item7.jpg',1)</v>
+        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(9,'CD','19 días y 500 noches','Joaquín Sabina',1990,'10','2','img/items/item7.jpg',1)</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -27860,8 +27869,8 @@
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>2</v>
+      <c r="C11" t="s">
+        <v>225</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>150</v>
@@ -27886,7 +27895,7 @@
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(10,2,'De vuelta y vuelta','Jarabe de Palo',2001,'1','1','img/items/item8.jpg',1)</v>
+        <v>INSERT INTO items (userID, itemType, title, artist, releaseYear, genreID, conditionID, image, available) VALUES(10,'CD','De vuelta y vuelta','Jarabe de Palo',2001,'1','1','img/items/item8.jpg',1)</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -27911,10 +27920,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
@@ -27934,7 +27943,7 @@
       <c r="B3" t="s">
         <v>218</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="21"/>
       <c r="D3" t="str">
         <f>CONCATENATE("INSERT INTO conditions (name) VALUES('",B3,"')")</f>
         <v>INSERT INTO conditions (name) VALUES('New')</v>
@@ -27984,10 +27993,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
     </row>
@@ -28148,7 +28157,7 @@
       </c>
     </row>
     <row r="21" spans="11:11">
-      <c r="K21" s="24"/>
+      <c r="K21" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -28171,13 +28180,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="12" t="s">
@@ -28224,10 +28233,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>

</xml_diff>